<commit_message>
first commit from eclipse
</commit_message>
<xml_diff>
--- a/robot/src/test/resources/data/out/loginTalan.xlsx
+++ b/robot/src/test/resources/data/out/loginTalan.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jsaidane\eclipse-workspace\robot\src\test\resources\data\out\"/>
     </mc:Choice>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>user</t>
   </si>
@@ -38,13 +38,17 @@
   </si>
   <si>
     <t>jihene123</t>
+  </si>
+  <si>
+    <t>Fail: /!\ Click on « talan.TALAN_PORTAL-menu » in talan. /!\</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -75,6 +79,21 @@
       <sz val="11"/>
       <color indexed="17"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="17"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="10"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="53"/>
     </font>
   </fonts>
   <fills count="4">
@@ -108,12 +127,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -437,7 +459,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -458,8 +480,8 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>4</v>
+      <c r="C2" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>